<commit_message>
falta solo lo binario
</commit_message>
<xml_diff>
--- a/UnitCommitment-T2/ResultadosCASE118-RES-90.xlsx
+++ b/UnitCommitment-T2/ResultadosCASE118-RES-90.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/vgoehringb_uc_cl/Documents/Ramos/Operación Economica/IEE3323--Operacion-Economica-Sistemas-Electricos/UnitCommitment-T2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="115_{0E09DC06-CFFD-4782-BD35-F7D2B8456CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADCDAF98-5BD2-4CD7-B2DC-D8E77CBDA351}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="115_{0E09DC06-CFFD-4782-BD35-F7D2B8456CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B50BE7-2056-4257-BF97-35CC19770373}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Potencias" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Costo Encendido</t>
   </si>
@@ -43,13 +43,99 @@
   <si>
     <t>END</t>
   </si>
+  <si>
+    <t>Hora 1</t>
+  </si>
+  <si>
+    <t>Hora 2</t>
+  </si>
+  <si>
+    <t>Hora 3</t>
+  </si>
+  <si>
+    <t>Hora 4</t>
+  </si>
+  <si>
+    <t>Hora 5</t>
+  </si>
+  <si>
+    <t>Hora 6</t>
+  </si>
+  <si>
+    <t>Hora 7</t>
+  </si>
+  <si>
+    <t>Hora 8</t>
+  </si>
+  <si>
+    <t>Hora 9</t>
+  </si>
+  <si>
+    <t>Hora 10</t>
+  </si>
+  <si>
+    <t>Hora 11</t>
+  </si>
+  <si>
+    <t>Hora 12</t>
+  </si>
+  <si>
+    <t>Hora 13</t>
+  </si>
+  <si>
+    <t>Hora 14</t>
+  </si>
+  <si>
+    <t>Hora 15</t>
+  </si>
+  <si>
+    <t>Hora 16</t>
+  </si>
+  <si>
+    <t>Hora 17</t>
+  </si>
+  <si>
+    <t>Hora 18</t>
+  </si>
+  <si>
+    <t>Hora 19</t>
+  </si>
+  <si>
+    <t>Hora 20</t>
+  </si>
+  <si>
+    <t>Hora 21</t>
+  </si>
+  <si>
+    <t>Hora 22</t>
+  </si>
+  <si>
+    <t>Hora 23</t>
+  </si>
+  <si>
+    <t>Hora 24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -77,8 +163,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -94,6 +181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8842,86 +8933,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEBE56D-35D4-43D7-B912-6460F4580581}">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X1" sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -9838,7 +9929,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -9912,7 +10003,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -9930,7 +10021,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -10004,7 +10095,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -10090,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -10131,7 +10222,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -10164,7 +10255,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -10202,10 +10293,10 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -10276,7 +10367,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -10312,7 +10403,7 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -10359,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -10386,7 +10477,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -10430,10 +10521,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -10504,10 +10595,10 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -10581,7 +10672,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -10608,7 +10699,7 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T24">
         <v>0</v>
@@ -10679,10 +10770,10 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25">
         <v>0</v>
@@ -10753,10 +10844,10 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <v>0</v>
@@ -10904,7 +10995,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -11129,7 +11220,7 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31">
         <v>0</v>
@@ -11277,7 +11368,7 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
         <v>0</v>
@@ -11351,7 +11442,7 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34">
         <v>0</v>
@@ -11425,10 +11516,10 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V35">
         <v>0</v>
@@ -11502,7 +11593,7 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -17287,97 +17378,172 @@
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+      <c r="T115">
+        <v>0</v>
+      </c>
+      <c r="U115">
+        <v>0</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115">
+        <v>0</v>
+      </c>
+      <c r="X115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A50DEC-A872-4489-89AA-78703A63ABD6}">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1">
-        <v>0</v>
-      </c>
-      <c r="N1">
-        <v>0</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -18561,7 +18727,7 @@
         <v>0</v>
       </c>
       <c r="X17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
@@ -18569,7 +18735,7 @@
         <v>0</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -18635,7 +18801,7 @@
         <v>0</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -18643,10 +18809,10 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -18720,7 +18886,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -18780,7 +18946,7 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -18854,7 +19020,7 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21">
         <v>0</v>
@@ -18928,7 +19094,7 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22">
         <v>0</v>
@@ -19076,10 +19242,10 @@
         <v>0</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
@@ -19153,7 +19319,7 @@
         <v>0</v>
       </c>
       <c r="X25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -19227,7 +19393,7 @@
         <v>0</v>
       </c>
       <c r="X26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -19298,10 +19464,10 @@
         <v>0</v>
       </c>
       <c r="W27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
@@ -19372,7 +19538,7 @@
         <v>0</v>
       </c>
       <c r="W28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X28">
         <v>0</v>
@@ -19594,7 +19760,7 @@
         <v>0</v>
       </c>
       <c r="W31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X31">
         <v>0</v>
@@ -19742,7 +19908,7 @@
         <v>0</v>
       </c>
       <c r="W33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X33">
         <v>0</v>
@@ -19813,7 +19979,7 @@
         <v>0</v>
       </c>
       <c r="V34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34">
         <v>0</v>
@@ -19961,7 +20127,7 @@
         <v>0</v>
       </c>
       <c r="V36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W36">
         <v>0</v>
@@ -25743,7 +25909,81 @@
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="A115">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+      <c r="T115">
+        <v>0</v>
+      </c>
+      <c r="U115">
+        <v>0</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115">
+        <v>0</v>
+      </c>
+      <c r="X115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>3</v>
       </c>
     </row>
@@ -25754,89 +25994,89 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD1C553-ECD3-4E53-9A56-5BFF99C76C22}">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" zoomScale="49" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-      <c r="J1">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>1</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>1</v>
-      </c>
-      <c r="N1">
-        <v>1</v>
-      </c>
-      <c r="O1">
-        <v>1</v>
-      </c>
-      <c r="P1">
-        <v>1</v>
-      </c>
-      <c r="Q1">
-        <v>1</v>
-      </c>
-      <c r="R1">
-        <v>1</v>
-      </c>
-      <c r="S1">
-        <v>1</v>
-      </c>
-      <c r="T1">
-        <v>1</v>
-      </c>
-      <c r="U1">
-        <v>1</v>
-      </c>
-      <c r="V1">
-        <v>1</v>
-      </c>
-      <c r="W1">
-        <v>1</v>
-      </c>
-      <c r="X1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -25910,7 +26150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -25984,7 +26224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -26058,7 +26298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -26132,7 +26372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -26206,7 +26446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -26280,7 +26520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -26354,7 +26594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -26428,7 +26668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -26502,7 +26742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -26576,7 +26816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -26650,7 +26890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -26724,30 +26964,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -26798,7 +27038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -26824,22 +27064,22 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -26872,48 +27112,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>1</v>
@@ -26945,61 +27185,62 @@
       <c r="X16">
         <v>1</v>
       </c>
+      <c r="AA16" s="1"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -27017,12 +27258,12 @@
         <v>1</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -27043,37 +27284,37 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -27091,7 +27332,7 @@
         <v>1</v>
       </c>
       <c r="X18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -27099,7 +27340,7 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -27114,7 +27355,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -27170,10 +27411,10 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -27188,40 +27429,40 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -27236,10 +27477,10 @@
         <v>1</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -27271,31 +27512,31 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21">
         <v>1</v>
@@ -27310,10 +27551,10 @@
         <v>1</v>
       </c>
       <c r="W21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -27342,7 +27583,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -27384,10 +27625,10 @@
         <v>1</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
@@ -27416,7 +27657,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -27493,31 +27734,31 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24">
         <v>1</v>
@@ -27532,7 +27773,7 @@
         <v>1</v>
       </c>
       <c r="W24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X24">
         <v>0</v>
@@ -27591,7 +27832,7 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25">
         <v>1</v>
@@ -27609,7 +27850,7 @@
         <v>1</v>
       </c>
       <c r="X25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -27665,7 +27906,7 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
         <v>1</v>
@@ -27683,7 +27924,7 @@
         <v>1</v>
       </c>
       <c r="X26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -27754,7 +27995,7 @@
         <v>1</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X27">
         <v>0</v>
@@ -27816,16 +28057,16 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W28">
         <v>0</v>
@@ -28041,13 +28282,13 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W31">
         <v>0</v>
@@ -28189,13 +28430,13 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33">
         <v>0</v>
@@ -28263,10 +28504,10 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -28337,7 +28578,7 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35">
         <v>1</v>
@@ -28414,7 +28655,7 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -29760,76 +30001,76 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
@@ -34199,7 +34440,81 @@
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115">
+        <v>1</v>
+      </c>
+      <c r="M115">
+        <v>1</v>
+      </c>
+      <c r="N115">
+        <v>1</v>
+      </c>
+      <c r="O115">
+        <v>1</v>
+      </c>
+      <c r="P115">
+        <v>1</v>
+      </c>
+      <c r="Q115">
+        <v>1</v>
+      </c>
+      <c r="R115">
+        <v>1</v>
+      </c>
+      <c r="S115">
+        <v>1</v>
+      </c>
+      <c r="T115">
+        <v>1</v>
+      </c>
+      <c r="U115">
+        <v>1</v>
+      </c>
+      <c r="V115">
+        <v>1</v>
+      </c>
+      <c r="W115">
+        <v>1</v>
+      </c>
+      <c r="X115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>